<commit_message>
adding info on cascadelake nodes
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
+++ b/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geert\Documents\Data\Projects\VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\HPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="0" windowWidth="16365" windowHeight="8760"/>
+    <workbookView xWindow="4760" yWindow="0" windowWidth="16370" windowHeight="8760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="201">
   <si>
     <t>r22g35</t>
   </si>
@@ -471,6 +471,183 @@
   </si>
   <si>
     <t>2.0 GHz</t>
+  </si>
+  <si>
+    <t>Xeon(R) Gold 6240</t>
+  </si>
+  <si>
+    <t>2.6 GHz</t>
+  </si>
+  <si>
+    <t>8 x V100</t>
+  </si>
+  <si>
+    <t>r25i27n01</t>
+  </si>
+  <si>
+    <t>r25i27n02</t>
+  </si>
+  <si>
+    <t>r25i27n03</t>
+  </si>
+  <si>
+    <t>r25i27n04</t>
+  </si>
+  <si>
+    <t>r25i27n05</t>
+  </si>
+  <si>
+    <t>r25i27n06</t>
+  </si>
+  <si>
+    <t>r25i27n07</t>
+  </si>
+  <si>
+    <t>r25i27n08</t>
+  </si>
+  <si>
+    <t>r25i27n09</t>
+  </si>
+  <si>
+    <t>r25i27n10</t>
+  </si>
+  <si>
+    <t>r25i27n11</t>
+  </si>
+  <si>
+    <t>r25i27n12</t>
+  </si>
+  <si>
+    <t>r25i27n13</t>
+  </si>
+  <si>
+    <t>r25i27n14</t>
+  </si>
+  <si>
+    <t>r25i27n15</t>
+  </si>
+  <si>
+    <t>r25i27n16</t>
+  </si>
+  <si>
+    <t>r25i27n17</t>
+  </si>
+  <si>
+    <t>r25i27n18</t>
+  </si>
+  <si>
+    <t>r25i27n19</t>
+  </si>
+  <si>
+    <t>r25i27n20</t>
+  </si>
+  <si>
+    <t>r25i27n21</t>
+  </si>
+  <si>
+    <t>r25i27n22</t>
+  </si>
+  <si>
+    <t>r25i27n23</t>
+  </si>
+  <si>
+    <t>r25i27n24</t>
+  </si>
+  <si>
+    <t>r26i27n01</t>
+  </si>
+  <si>
+    <t>r26i27n13</t>
+  </si>
+  <si>
+    <t>r26i27n02</t>
+  </si>
+  <si>
+    <t>r26i27n03</t>
+  </si>
+  <si>
+    <t>r26i27n04</t>
+  </si>
+  <si>
+    <t>r26i27n05</t>
+  </si>
+  <si>
+    <t>r26i27n06</t>
+  </si>
+  <si>
+    <t>r26i27n07</t>
+  </si>
+  <si>
+    <t>r26i27n08</t>
+  </si>
+  <si>
+    <t>r26i27n09</t>
+  </si>
+  <si>
+    <t>r26i27n10</t>
+  </si>
+  <si>
+    <t>r26i27n11</t>
+  </si>
+  <si>
+    <t>r26i27n12</t>
+  </si>
+  <si>
+    <t>r26i27n14</t>
+  </si>
+  <si>
+    <t>r26i27n15</t>
+  </si>
+  <si>
+    <t>r26i27n16</t>
+  </si>
+  <si>
+    <t>r26i27n17</t>
+  </si>
+  <si>
+    <t>r26i27n18</t>
+  </si>
+  <si>
+    <t>r26i27n19</t>
+  </si>
+  <si>
+    <t>r26i27n20</t>
+  </si>
+  <si>
+    <t>r26i27n21</t>
+  </si>
+  <si>
+    <t>r26i27n22</t>
+  </si>
+  <si>
+    <t>r26i27n23</t>
+  </si>
+  <si>
+    <t>r26i27n24</t>
+  </si>
+  <si>
+    <t>r26i13n01</t>
+  </si>
+  <si>
+    <t>r26i13n13</t>
+  </si>
+  <si>
+    <t>r27i27n01</t>
+  </si>
+  <si>
+    <t>r27i27n13</t>
+  </si>
+  <si>
+    <t>r25i13n01</t>
+  </si>
+  <si>
+    <t>r25i13n13</t>
+  </si>
+  <si>
+    <t>r24g05</t>
+  </si>
+  <si>
+    <t>r24g09</t>
   </si>
 </sst>
 </file>
@@ -531,7 +708,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,18 +735,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -634,13 +817,33 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -655,7 +858,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -667,10 +870,10 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thick">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -679,7 +882,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thick">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -688,7 +891,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -703,7 +906,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -712,65 +915,58 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thick">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,18 +1250,18 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:L35"/>
+  <dimension ref="A4:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1088,489 +1284,898 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="17" t="s">
+      <c r="J6" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="17" t="s">
+      <c r="K6" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="18" t="s">
+      <c r="L6" s="31" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="12" t="s">
+      <c r="L8" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="K11" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="8" t="s">
+      <c r="J12" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="8" t="s">
+      <c r="K12" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="L12" s="28" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="35" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="I14" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+    <row r="15" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="J17" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="K18" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="K19" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="K20" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="J21" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="K21" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="L21" s="21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>187</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="J22" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="L23" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="J24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="K24" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B25" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C25" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D25" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E19" s="30"/>
-      <c r="G19" t="s">
+    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="10"/>
+      <c r="C28" t="s">
         <v>132</v>
       </c>
-      <c r="H19" t="s">
+      <c r="D28" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G22" s="20" t="s">
+      <c r="G28" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20" t="s">
+      <c r="H28" s="5"/>
+      <c r="I28" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J28" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="K22" s="20" t="s">
+      <c r="K28" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="L28" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E23" s="19"/>
-      <c r="G23" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E29" s="18"/>
+      <c r="G29" t="s">
         <v>122</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I29" t="s">
         <v>124</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J29" t="s">
         <v>126</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K29" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="3"/>
-      <c r="G25" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C30" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="G30" t="s">
         <v>122</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I30" t="s">
         <v>124</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J30" t="s">
         <v>126</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K30" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E27" s="1"/>
-      <c r="G27" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="15"/>
+      <c r="G31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I31" t="s">
+        <v>143</v>
+      </c>
+      <c r="J31" t="s">
+        <v>126</v>
+      </c>
+      <c r="K31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="G32" t="s">
         <v>122</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I32" t="s">
         <v>124</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J32" t="s">
         <v>126</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K32" t="s">
         <v>118</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L32" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E29" s="31"/>
-      <c r="G29" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="G33" t="s">
+        <v>142</v>
+      </c>
+      <c r="I33" t="s">
+        <v>143</v>
+      </c>
+      <c r="J33" t="s">
+        <v>126</v>
+      </c>
+      <c r="K33" t="s">
+        <v>118</v>
+      </c>
+      <c r="L33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E34" s="11"/>
+      <c r="G34" t="s">
         <v>138</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I34" t="s">
         <v>141</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J34" t="s">
         <v>139</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K34" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E33" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="G33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="96" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update genius node map with debug thin nodes
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
+++ b/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\HPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\VscDocumentation\source\leuven\tier2_hardware\genius_hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E12731-9F17-4DE5-B032-DF71D12B7058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="0" windowWidth="16370" windowHeight="8760"/>
+    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -653,8 +654,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,14 +667,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -707,8 +700,48 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -751,6 +784,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -930,21 +969,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -957,16 +992,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1246,22 +1289,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:L34"/>
+  <dimension ref="A4:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1284,163 +1327,163 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25" t="s">
+    <row r="5" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="I5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="29" t="s">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="30" t="s">
+      <c r="I6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="30" t="s">
+      <c r="J6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="K6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="31" t="s">
+      <c r="L6" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="30" t="s">
+      <c r="J8" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="K8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="31" t="s">
+      <c r="L8" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="31" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1456,163 +1499,164 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="27" t="s">
+      <c r="G10" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="27" t="s">
+      <c r="H10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="27" t="s">
+      <c r="I10" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="L10" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="31" t="s">
+      <c r="L11" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="28" t="s">
+      <c r="L12" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="29" t="s">
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="33" t="s">
+      <c r="F13" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="33" t="s">
+      <c r="G13" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="33" t="s">
+      <c r="I13" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="34" t="s">
+      <c r="J13" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="35" t="s">
+      <c r="L13" s="36" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="16" t="s">
+      <c r="N13" s="34"/>
+    </row>
+    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="13" t="s">
         <v>200</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1633,407 +1677,407 @@
       <c r="H14" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="K15" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="L15" s="21" t="s">
+      <c r="L15" s="17" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="22" t="s">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="L16" s="20" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="F17" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H17" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I17" s="20" t="s">
+      <c r="I17" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="20" t="s">
+      <c r="K17" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="L17" s="21" t="s">
+      <c r="L17" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="23" t="s">
+      <c r="D18" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="H18" s="23" t="s">
+      <c r="H18" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="I18" s="23" t="s">
+      <c r="I18" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="K19" s="20" t="s">
+      <c r="K19" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="17" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="I20" s="23" t="s">
+      <c r="I20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="K20" s="23" t="s">
+      <c r="K20" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="L20" s="24" t="s">
+      <c r="L20" s="20" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="H21" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="L21" s="21" t="s">
+      <c r="L21" s="17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="22" t="s">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="D22" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="I22" s="23" t="s">
+      <c r="I22" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="K22" s="23" t="s">
+      <c r="K22" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="L22" s="24" t="s">
+      <c r="L22" s="20" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="K23" s="20" t="s">
+      <c r="K23" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="L23" s="21" t="s">
+      <c r="L23" s="17" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="22" t="s">
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="D24" s="23" t="s">
+      <c r="D24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="I24" s="23" t="s">
+      <c r="I24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="K24" s="23" t="s">
+      <c r="K24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="L24" s="20" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="s">
+    <row r="25" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="10"/>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
       <c r="C28" t="s">
         <v>132</v>
       </c>
@@ -2057,8 +2101,8 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E29" s="18"/>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E29" s="14"/>
       <c r="G29" t="s">
         <v>122</v>
       </c>
@@ -2072,8 +2116,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C30" s="5" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
         <v>131</v>
       </c>
       <c r="E30" s="3"/>
@@ -2090,14 +2134,14 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B31" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="15"/>
+      <c r="E31" s="11"/>
       <c r="G31" t="s">
         <v>142</v>
       </c>
@@ -2111,11 +2155,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A32" s="8" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B32" t="s">
         <v>129</v>
       </c>
       <c r="E32" s="1"/>
@@ -2135,14 +2179,14 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C33" t="s">
+      <c r="B33" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="8"/>
       <c r="G33" t="s">
         <v>142</v>
       </c>
@@ -2159,8 +2203,8 @@
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E34" s="11"/>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E34" s="7"/>
       <c r="G34" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Update nodemap wrt Cascadelake & V100 upgrades
</commit_message>
<xml_diff>
--- a/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
+++ b/source/leuven/tier2_hardware/genius_hardware/genius_node_map.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\VscDocumentation\source\leuven\tier2_hardware\genius_hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0137498\Documents\misc\vsc_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E12731-9F17-4DE5-B032-DF71D12B7058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-120" windowWidth="27855" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="291">
   <si>
     <t>r22g35</t>
   </si>
@@ -650,11 +649,281 @@
   <si>
     <t>r24g09</t>
   </si>
+  <si>
+    <t>r27i13n01</t>
+  </si>
+  <si>
+    <t>r27i13n02</t>
+  </si>
+  <si>
+    <t>r27i13n03</t>
+  </si>
+  <si>
+    <t>r27i13n04</t>
+  </si>
+  <si>
+    <t>r27i13n05</t>
+  </si>
+  <si>
+    <t>r27i13n06</t>
+  </si>
+  <si>
+    <t>r27i13n07</t>
+  </si>
+  <si>
+    <t>r27i13n08</t>
+  </si>
+  <si>
+    <t>r27i13n09</t>
+  </si>
+  <si>
+    <t>r27i13n10</t>
+  </si>
+  <si>
+    <t>r27i13n11</t>
+  </si>
+  <si>
+    <t>r27i13n12</t>
+  </si>
+  <si>
+    <t>r27i13n13</t>
+  </si>
+  <si>
+    <t>r27i13n14</t>
+  </si>
+  <si>
+    <t>r27i13n15</t>
+  </si>
+  <si>
+    <t>r27i13n16</t>
+  </si>
+  <si>
+    <t>r27i13n17</t>
+  </si>
+  <si>
+    <t>r27i13n18</t>
+  </si>
+  <si>
+    <t>r27i13n19</t>
+  </si>
+  <si>
+    <t>r27i13n20</t>
+  </si>
+  <si>
+    <t>r27i13n21</t>
+  </si>
+  <si>
+    <t>r27i13n22</t>
+  </si>
+  <si>
+    <t>r27i13n23</t>
+  </si>
+  <si>
+    <t>r27i27n12</t>
+  </si>
+  <si>
+    <t>r27i27n24</t>
+  </si>
+  <si>
+    <t>r27i27n14</t>
+  </si>
+  <si>
+    <t>r27i27n15</t>
+  </si>
+  <si>
+    <t>r27i27n16</t>
+  </si>
+  <si>
+    <t>r27i27n17</t>
+  </si>
+  <si>
+    <t>r27i27n18</t>
+  </si>
+  <si>
+    <t>r27i27n19</t>
+  </si>
+  <si>
+    <t>r27i27n20</t>
+  </si>
+  <si>
+    <t>r27i27n21</t>
+  </si>
+  <si>
+    <t>r27i27n22</t>
+  </si>
+  <si>
+    <t>r27i27n23</t>
+  </si>
+  <si>
+    <t>r27i13n24</t>
+  </si>
+  <si>
+    <t>r27i27n02</t>
+  </si>
+  <si>
+    <t>r27i27n03</t>
+  </si>
+  <si>
+    <t>r27i27n04</t>
+  </si>
+  <si>
+    <t>r27i27n05</t>
+  </si>
+  <si>
+    <t>r27i27n06</t>
+  </si>
+  <si>
+    <t>r27i27n07</t>
+  </si>
+  <si>
+    <t>r27i27n08</t>
+  </si>
+  <si>
+    <t>r27i27n09</t>
+  </si>
+  <si>
+    <t>r27i27n10</t>
+  </si>
+  <si>
+    <t>r27i27n11</t>
+  </si>
+  <si>
+    <t>r26i13n02</t>
+  </si>
+  <si>
+    <t>r26i13n03</t>
+  </si>
+  <si>
+    <t>r26i13n04</t>
+  </si>
+  <si>
+    <t>r26i13n05</t>
+  </si>
+  <si>
+    <t>r26i13n06</t>
+  </si>
+  <si>
+    <t>r26i13n07</t>
+  </si>
+  <si>
+    <t>r26i13n08</t>
+  </si>
+  <si>
+    <t>r26i13n09</t>
+  </si>
+  <si>
+    <t>r26i13n10</t>
+  </si>
+  <si>
+    <t>r26i13n11</t>
+  </si>
+  <si>
+    <t>r26i13n12</t>
+  </si>
+  <si>
+    <t>r26i13n14</t>
+  </si>
+  <si>
+    <t>r26i13n15</t>
+  </si>
+  <si>
+    <t>r26i13n16</t>
+  </si>
+  <si>
+    <t>r26i13n17</t>
+  </si>
+  <si>
+    <t>r26i13n18</t>
+  </si>
+  <si>
+    <t>r26i13n19</t>
+  </si>
+  <si>
+    <t>r26i13n20</t>
+  </si>
+  <si>
+    <t>r26i13n21</t>
+  </si>
+  <si>
+    <t>r26i13n22</t>
+  </si>
+  <si>
+    <t>r26i13n23</t>
+  </si>
+  <si>
+    <t>r26i13n24</t>
+  </si>
+  <si>
+    <t>r25i13n02</t>
+  </si>
+  <si>
+    <t>r25i13n03</t>
+  </si>
+  <si>
+    <t>r25i13n04</t>
+  </si>
+  <si>
+    <t>r25i13n05</t>
+  </si>
+  <si>
+    <t>r25i13n06</t>
+  </si>
+  <si>
+    <t>r25i13n07</t>
+  </si>
+  <si>
+    <t>r25i13n08</t>
+  </si>
+  <si>
+    <t>r25i13n09</t>
+  </si>
+  <si>
+    <t>r25i13n10</t>
+  </si>
+  <si>
+    <t>r25i13n11</t>
+  </si>
+  <si>
+    <t>r25i13n12</t>
+  </si>
+  <si>
+    <t>r25i13n14</t>
+  </si>
+  <si>
+    <t>r25i13n15</t>
+  </si>
+  <si>
+    <t>r25i13n16</t>
+  </si>
+  <si>
+    <t>r25i13n17</t>
+  </si>
+  <si>
+    <t>r25i13n18</t>
+  </si>
+  <si>
+    <t>r25i13n19</t>
+  </si>
+  <si>
+    <t>r25i13n20</t>
+  </si>
+  <si>
+    <t>r25i13n21</t>
+  </si>
+  <si>
+    <t>r25i13n22</t>
+  </si>
+  <si>
+    <t>r25i13n23</t>
+  </si>
+  <si>
+    <t>r25i13n24</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1012,7 +1281,7 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1289,937 +1558,1013 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A4:N34"/>
+  <dimension ref="B4:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="D5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="E5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="F5" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="H5" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="I5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="J5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="K5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="L5" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="M5" s="23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="E6" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="F6" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="I6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="J6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="K6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="25" t="s">
+      <c r="L6" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="26" t="s">
+      <c r="M6" s="26" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="C7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="E7" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="F7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="G7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="H7" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="I7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="K7" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="L7" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="M7" s="23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+    <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="D8" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="F8" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="G8" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="H8" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="I8" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="J8" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="K8" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="L8" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="M8" s="26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="C9" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+    <row r="10" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="C10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="D10" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="E10" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="F10" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="G10" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="H10" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="I10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="J10" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="22" t="s">
+      <c r="K10" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="L10" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="M10" s="23" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="C11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="D11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="E11" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="F11" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="G11" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="H11" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="I11" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="J11" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="K11" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="L11" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="L11" s="26" t="s">
+      <c r="M11" s="26" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+    <row r="12" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="C12" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="D12" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="E12" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="F12" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="G12" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="H12" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="I12" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="J12" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="K12" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="L12" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="M12" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="C13" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="D13" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="E13" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="F13" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="G13" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="H13" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="H13" s="28" t="s">
+      <c r="I13" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="J13" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="K13" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="L13" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="36" t="s">
+      <c r="M13" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="1:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="C14" s="13" t="s">
         <v>200</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="H14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="J14" s="9" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="2:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>197</v>
-      </c>
       <c r="C15" s="16" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>197</v>
+        <v>270</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>197</v>
+        <v>271</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>197</v>
+        <v>272</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>197</v>
+        <v>273</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>197</v>
+        <v>275</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>197</v>
+        <v>276</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>198</v>
-      </c>
       <c r="C16" s="19" t="s">
-        <v>198</v>
+        <v>280</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>198</v>
+        <v>281</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>198</v>
+        <v>282</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>198</v>
+        <v>283</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
       <c r="H16" s="19" t="s">
-        <v>198</v>
+        <v>285</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>198</v>
+        <v>287</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="M16" s="20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="E17" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="F17" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="G17" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="H17" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="H17" s="16" t="s">
+      <c r="I17" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="I17" s="16" t="s">
+      <c r="J17" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="J17" s="16" t="s">
+      <c r="K17" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="L17" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="L17" s="17" t="s">
+      <c r="M17" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="D18" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="E18" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="F18" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="G18" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="I18" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="J18" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="K18" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="L18" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="L18" s="20" t="s">
+      <c r="M18" s="20" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>193</v>
-      </c>
       <c r="C19" s="16" t="s">
-        <v>193</v>
+        <v>247</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>193</v>
+        <v>249</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>193</v>
+        <v>250</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>193</v>
+        <v>253</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>193</v>
+        <v>254</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>193</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>194</v>
-      </c>
       <c r="C20" s="19" t="s">
-        <v>194</v>
+        <v>258</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>194</v>
+        <v>259</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>194</v>
+        <v>260</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>194</v>
+        <v>262</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>194</v>
+        <v>263</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>194</v>
+        <v>264</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>194</v>
+        <v>265</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="L20" s="20" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="L20" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="M20" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="D21" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="E21" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="G21" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="H21" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="I21" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="J21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="J21" s="16" t="s">
+      <c r="K21" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="L21" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="L21" s="17" t="s">
+      <c r="M21" s="17" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
+    <row r="22" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="D22" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="E22" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="G22" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="H22" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="I22" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="J22" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="K22" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="K22" s="19" t="s">
+      <c r="L22" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="L22" s="20" t="s">
+      <c r="M22" s="20" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="J24" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="L24" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="M24" s="20" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="K23" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="L23" s="17" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="C25" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="L25" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="M25" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="H24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="K24" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="C26" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="L26" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="M26" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="C27" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="C28" t="s">
+    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="6"/>
+      <c r="D30" t="s">
         <v>132</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E30" t="s">
         <v>133</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5" t="s">
+      <c r="I30" s="5"/>
+      <c r="J30" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="K30" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="L30" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="L28" s="5" t="s">
+      <c r="M30" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E29" s="14"/>
-      <c r="G29" t="s">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F31" s="14"/>
+      <c r="H31" t="s">
         <v>122</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J31" t="s">
         <v>124</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K31" t="s">
         <v>126</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L31" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C32" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="G30" t="s">
+      <c r="F32" s="3"/>
+      <c r="H32" t="s">
         <v>122</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J32" t="s">
         <v>124</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K32" t="s">
         <v>126</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L32" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="37" t="s">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C33" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="G31" t="s">
+      <c r="F33" s="11"/>
+      <c r="H33" t="s">
         <v>142</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J33" t="s">
         <v>143</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K33" t="s">
         <v>126</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C34" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="G32" t="s">
+      <c r="F34" s="1"/>
+      <c r="H34" t="s">
         <v>122</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J34" t="s">
         <v>124</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K34" t="s">
         <v>126</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L34" t="s">
         <v>118</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="39" t="s">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C35" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="G33" t="s">
+      <c r="F35" s="8"/>
+      <c r="H35" t="s">
         <v>142</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J35" t="s">
         <v>143</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K35" t="s">
         <v>126</v>
       </c>
-      <c r="K33" t="s">
-        <v>118</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="L35" t="s">
+        <v>119</v>
+      </c>
+      <c r="M35" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E34" s="7"/>
-      <c r="G34" t="s">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F36" s="7"/>
+      <c r="H36" t="s">
         <v>138</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J36" t="s">
         <v>141</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K36" t="s">
         <v>139</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L36" t="s">
         <v>140</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>